<commit_message>
feat: Implement initial PMET analysis reporting with HTML summary, data, and Excel report files.
</commit_message>
<xml_diff>
--- a/Koudaya/Rapport_Analyse_PMET_Simple.xlsx
+++ b/Koudaya/Rapport_Analyse_PMET_Simple.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Type PMET</t>
   </si>
@@ -46,10 +46,7 @@
     <t>G PMET</t>
   </si>
   <si>
-    <t>09/01/2026 14:29</t>
-  </si>
-  <si>
-    <t>09/01/2026 14:30</t>
+    <t>12/01/2026 09:56</t>
   </si>
 </sst>
 </file>
@@ -488,7 +485,7 @@
         <v>20.625</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>